<commit_message>
add multi summary sheets
</commit_message>
<xml_diff>
--- a/dataset/models/input/OperationsConstants.xlsx
+++ b/dataset/models/input/OperationsConstants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminkauffmann/Desktop/Azasimul/azasimul/dataset/models/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2BEA19C-53C7-3C4A-B7BA-0D1704697075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E911E7F-BB9D-8C40-963C-F33C26AA2A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="500" windowWidth="26760" windowHeight="8500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9260" yWindow="9300" windowWidth="26760" windowHeight="8500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operations" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="86">
   <si>
     <t>Global constants</t>
   </si>
@@ -377,6 +377,36 @@
   <si>
     <t>{BatteryPack.Weight}*[BatteryPack Quantity]</t>
   </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nameplate Load </t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>Project Duration Yearly</t>
+  </si>
+  <si>
+    <t>Project Duration Monthly</t>
+  </si>
+  <si>
+    <t>Annual MWh delivered</t>
+  </si>
+  <si>
+    <t>Project MWh delivered</t>
+  </si>
+  <si>
+    <t>Market</t>
+  </si>
+  <si>
+    <t>Real WACC</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
 </sst>
 </file>
 
@@ -387,7 +417,7 @@
     <numFmt numFmtId="165" formatCode="#,##0%"/>
     <numFmt numFmtId="166" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -442,6 +472,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -514,7 +552,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -577,6 +615,14 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -884,10 +930,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -899,294 +945,354 @@
     <col min="5" max="7" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B2" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="22"/>
+      <c r="B5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="22"/>
+      <c r="B6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="22"/>
+      <c r="B7"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="22"/>
+      <c r="B10"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="19"/>
+    </row>
+    <row r="11" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="14"/>
-      <c r="C6" s="11"/>
-    </row>
-    <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" s="20"/>
-    </row>
-    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="2"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>58</v>
+        <v>37</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>61</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>64</v>
+        <v>4</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
       <c r="B15" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>66</v>
+      <c r="C15" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="18"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B19" s="4"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="14"/>
+      <c r="C16" s="11"/>
+    </row>
+    <row r="17" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G19" s="20"/>
+    </row>
+    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="21" t="s">
-        <v>37</v>
-      </c>
       <c r="C21" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-      <c r="B22" s="21" t="s">
-        <v>40</v>
+        <v>56</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="21"/>
-    </row>
-    <row r="24" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="21"/>
-    </row>
-    <row r="25" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
+        <v>58</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>68</v>
+      </c>
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="11"/>
+    <row r="27" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>70</v>
+      </c>
       <c r="D27" s="4"/>
     </row>
-    <row r="28" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
+    <row r="28" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="18"/>
       <c r="D28" s="4"/>
     </row>
-    <row r="29" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
+    <row r="29" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="B29" s="4"/>
       <c r="D29" s="4"/>
     </row>
-    <row r="30" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="14"/>
-    </row>
-    <row r="31" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="4"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="4"/>
-    </row>
-    <row r="32" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="14"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="4"/>
-    </row>
-    <row r="33" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="14"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="4"/>
+    <row r="30" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
+      <c r="B32" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="21"/>
+    </row>
+    <row r="34" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="4"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="21"/>
+    </row>
+    <row r="35" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="14"/>
+    </row>
+    <row r="41" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="4"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="4"/>
+    </row>
+    <row r="42" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="14"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="4"/>
+    </row>
+    <row r="43" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="14"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add : take into account summary datas
</commit_message>
<xml_diff>
--- a/dataset/models/input/OperationsConstants.xlsx
+++ b/dataset/models/input/OperationsConstants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminkauffmann/Desktop/Azasimul/azasimul/dataset/models/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F112DF70-F107-8244-B7D5-F9748CB01904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68613B5A-2DFC-004D-A171-6F7CC01C1714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9520" yWindow="8340" windowWidth="26760" windowHeight="8500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="88">
   <si>
     <t>Global constants</t>
   </si>
@@ -409,6 +409,9 @@
   </si>
   <si>
     <t>[Summary.End]-[Summary.Start]</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
@@ -944,7 +947,7 @@
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -975,6 +978,9 @@
       </c>
       <c r="C3" s="26" t="s">
         <v>86</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add: filters for date's calculations
</commit_message>
<xml_diff>
--- a/dataset/models/input/OperationsConstants.xlsx
+++ b/dataset/models/input/OperationsConstants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminkauffmann/Desktop/Azasimul/azasimul/dataset/models/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68613B5A-2DFC-004D-A171-6F7CC01C1714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269CB2C9-E6BB-C742-A6AF-74CF7EE854EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9520" yWindow="8340" windowWidth="26760" windowHeight="8500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9600" yWindow="7360" windowWidth="26760" windowHeight="8500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operations" sheetId="1" r:id="rId1"/>
@@ -408,10 +408,10 @@
     <t>%</t>
   </si>
   <si>
-    <t>[Summary.End]-[Summary.Start]</t>
-  </si>
-  <si>
-    <t>date</t>
+    <t>{Project Duration Yearly}*12</t>
+  </si>
+  <si>
+    <t>[Summary.End|year]-[Summary.Start|year]</t>
   </si>
 </sst>
 </file>
@@ -977,9 +977,6 @@
         <v>79</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="D3" s="19" t="s">
         <v>87</v>
       </c>
     </row>
@@ -987,7 +984,9 @@
       <c r="B4" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="26"/>
+      <c r="C4" s="26" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="22"/>
@@ -1327,7 +1326,7 @@
   </sheetPr>
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>